<commit_message>
Week 6 - Corrected Configuration Items List
</commit_message>
<xml_diff>
--- a/Configuration Items List v2.0.xlsx
+++ b/Configuration Items List v2.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Keith's Documents\BU - MSIT\CS633 - Distributed Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kbennett\Documents\GitHub\CSS633---Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -730,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H58"/>
+  <dimension ref="B1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1473,7 +1473,7 @@
       <c r="B24" s="2">
         <v>19</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="20" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="4">
@@ -1562,7 +1562,9 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <v>23</v>
+      </c>
       <c r="C28" s="20" t="s">
         <v>50</v>
       </c>
@@ -1583,7 +1585,9 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
+      <c r="B29" s="2">
+        <v>24</v>
+      </c>
       <c r="C29" s="20" t="s">
         <v>51</v>
       </c>
@@ -1604,7 +1608,9 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
+      <c r="B30" s="2">
+        <v>25</v>
+      </c>
       <c r="C30" s="20" t="s">
         <v>52</v>
       </c>
@@ -1625,7 +1631,9 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
+      <c r="B31" s="2">
+        <v>26</v>
+      </c>
       <c r="C31" s="20" t="s">
         <v>53</v>
       </c>
@@ -1646,7 +1654,9 @@
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
+      <c r="B32" s="2">
+        <v>27</v>
+      </c>
       <c r="C32" s="20" t="s">
         <v>54</v>
       </c>
@@ -1667,7 +1677,9 @@
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
+      <c r="B33" s="2">
+        <v>28</v>
+      </c>
       <c r="C33" s="20" t="s">
         <v>56</v>
       </c>
@@ -1688,7 +1700,9 @@
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="2"/>
+      <c r="B34" s="2">
+        <v>29</v>
+      </c>
       <c r="C34" s="20" t="s">
         <v>57</v>
       </c>
@@ -1709,7 +1723,9 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="2"/>
+      <c r="B35" s="2">
+        <v>30</v>
+      </c>
       <c r="C35" s="20" t="s">
         <v>68</v>
       </c>
@@ -1730,7 +1746,9 @@
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="2"/>
+      <c r="B36" s="2">
+        <v>31</v>
+      </c>
       <c r="C36" s="20" t="s">
         <v>59</v>
       </c>
@@ -1751,7 +1769,9 @@
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="2"/>
+      <c r="B37" s="2">
+        <v>32</v>
+      </c>
       <c r="C37" s="20" t="s">
         <v>61</v>
       </c>
@@ -1772,7 +1792,9 @@
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="2"/>
+      <c r="B38" s="2">
+        <v>33</v>
+      </c>
       <c r="C38" s="20" t="s">
         <v>62</v>
       </c>
@@ -1793,7 +1815,9 @@
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="2"/>
+      <c r="B39" s="2">
+        <v>34</v>
+      </c>
       <c r="C39" s="20" t="s">
         <v>63</v>
       </c>
@@ -1814,7 +1838,9 @@
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
+      <c r="B40" s="2">
+        <v>35</v>
+      </c>
       <c r="C40" s="20" t="s">
         <v>64</v>
       </c>
@@ -1835,7 +1861,9 @@
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="2"/>
+      <c r="B41" s="2">
+        <v>36</v>
+      </c>
       <c r="C41" s="20" t="s">
         <v>65</v>
       </c>
@@ -1856,7 +1884,9 @@
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="2"/>
+      <c r="B42" s="2">
+        <v>37</v>
+      </c>
       <c r="C42" s="20" t="s">
         <v>66</v>
       </c>
@@ -1877,7 +1907,9 @@
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="2"/>
+      <c r="B43" s="2">
+        <v>38</v>
+      </c>
       <c r="C43" s="20" t="s">
         <v>67</v>
       </c>
@@ -1906,95 +1938,23 @@
       <c r="G44" s="2"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="2"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="2"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="7"/>
-    </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="2"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="7"/>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="2"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="2"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="2"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="7"/>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="2"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+      <c r="C48" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2039,6 +1999,7 @@
     <hyperlink ref="C43" r:id="rId34"/>
     <hyperlink ref="C35" r:id="rId35"/>
     <hyperlink ref="C10" r:id="rId36"/>
+    <hyperlink ref="C24" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>